<commit_message>
corrections in template parsers
</commit_message>
<xml_diff>
--- a/microservices/download templates/src/templatesStorage/templates_original/LineWithAnnotationsTemplate.xlsx
+++ b/microservices/download templates/src/templatesStorage/templates_original/LineWithAnnotationsTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DORA\Documents\GitHub\SaaS23-60\microservices\download templates\src\templatesStorage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DORA\Documents\GitHub\SaaS23-60\microservices\download templates\src\templatesStorage\templates_original\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C89A97-65D8-48FC-BE09-21BBDC49FA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597BA496-D4BD-4CCE-9943-227AD1380D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{46EB44D5-4E4C-4FBF-9B9B-9B8682C03FE5}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:BY462"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6544,7 +6544,7 @@
       <c r="BY462" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="VEWD6HVC5JhfM6UiGdSTXOVH2jt087kGG4WBiwMUqdKV8KwPnuEfo1TW3wIsELftEIVn+I2weKxhWbkzzg5opA==" saltValue="wWiK+n1zvtlP9OVTv/p5hQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="4+Ep1CSoQ8nJuRsmDYZVvPUAZDhksShAeg+BcKfR6mHlic9VRRo61xais4mAtC4B/POho1XxxuKrfnwvrnXJyw==" saltValue="7WJOJOX5IstciYTglESWzQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="grJ6j9Pg3fR0ozyFbWId1iGPDl+m/wcgohlsBFVdFPlu3vLW2Q2diNvdtQZ4Y/z885xl+QQPzwXqYSHB89EeWw==" saltValue="Iwv+UuEJEwdeanhrSECMnw==" spinCount="100000" sqref="A1:XFD2" name="Range1"/>
   </protectedRanges>
@@ -6554,8 +6554,8 @@
   <dataValidations count="4">
     <dataValidation showInputMessage="1" showErrorMessage="1" error="Needs to be in &quot;number&quot; - &quot;number&quot; format_x000a_" prompt="Write the measurement unit for x Axis. E.g km,meters,..." sqref="D3" xr:uid="{6C8AAD9E-B5B6-4F21-B492-A65D1B8513F2}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the measurement unit for y Axis. E.g km,meters,..." sqref="E3" xr:uid="{E73B49D8-1172-4147-BFE1-F35B0D15AB4C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write it in the format x y !" sqref="F6" xr:uid="{8FCDBCBB-3A6E-4A7D-9A39-12402BE3E2E9}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write it in the format x y!" sqref="D6" xr:uid="{880FB2AC-3643-42A6-80F9-DC8B77A6DAE4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write it in the format:_x000a_x y_x000a_Where (x,y) is the point the label will be shown." sqref="F6" xr:uid="{8FCDBCBB-3A6E-4A7D-9A39-12402BE3E2E9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write it in the format:_x000a_x y_x000a_Where (x,y) is the point the label will be shown." sqref="D6" xr:uid="{880FB2AC-3643-42A6-80F9-DC8B77A6DAE4}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>